<commit_message>
Prevent division by zero error in city_economic_calc.py for CHP usage
</commit_message>
<xml_diff>
--- a/pycity_calc/cities/scripts/city_generator/input/city_3_buildings.xlsx
+++ b/pycity_calc/cities/scripts/city_generator/input/city_3_buildings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arbeitsordner_Lokal\PyCharm_workspace\pycity_calc\pycity_calc\cities\scripts\city_generator\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arbeitsordner_Lokal\PyCharm_workspace\pyCity_calc\pycity_calc\cities\scripts\city_generator\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -950,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,18 +1056,15 @@
         <v>0</v>
       </c>
       <c r="E2" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="F2" s="1">
         <v>1980</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="1">
-        <f t="shared" ref="H2" si="0">E2*150</f>
-        <v>15000</v>
-      </c>
-      <c r="I2">
-        <v>2500</v>
+      <c r="H2" s="1"/>
+      <c r="J2">
+        <v>0</v>
       </c>
       <c r="K2" s="1">
         <v>1</v>
@@ -1117,7 +1114,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>150</v>
+        <v>400</v>
       </c>
       <c r="F3" s="1">
         <v>1980</v>
@@ -1132,7 +1129,7 @@
         <v>2</v>
       </c>
       <c r="L3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M3">
         <v>2</v>
@@ -1176,7 +1173,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>125</v>
+        <v>300</v>
       </c>
       <c r="F4" s="1">
         <v>1980</v>
@@ -1184,12 +1181,8 @@
       <c r="G4" s="1">
         <v>2014</v>
       </c>
-      <c r="H4" s="1">
-        <v>10000</v>
-      </c>
-      <c r="I4" s="1">
-        <v>3200</v>
-      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
       <c r="J4" s="1">
         <v>30</v>
       </c>

</xml_diff>